<commit_message>
Edit my list by new reference
</commit_message>
<xml_diff>
--- a/Document/DPV.ATL/Attribute List.xlsx
+++ b/Document/DPV.ATL/Attribute List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="18" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="BankAccount" sheetId="27" r:id="rId1"/>
@@ -28,36 +28,37 @@
     <sheet name="CustomerShipAddress" sheetId="26" r:id="rId19"/>
     <sheet name="DeliveryPerson" sheetId="44" r:id="rId20"/>
     <sheet name="DiscountCode" sheetId="45" r:id="rId21"/>
-    <sheet name="Manufacture" sheetId="46" r:id="rId22"/>
-    <sheet name="Product" sheetId="1" r:id="rId23"/>
-    <sheet name="ProductBase" sheetId="8" r:id="rId24"/>
-    <sheet name="ProductBaseProductMap" sheetId="9" r:id="rId25"/>
-    <sheet name="ProductComment" sheetId="7" r:id="rId26"/>
-    <sheet name="ProductGroup" sheetId="6" r:id="rId27"/>
-    <sheet name="ProductPicture" sheetId="5" r:id="rId28"/>
-    <sheet name="ProductRate" sheetId="10" r:id="rId29"/>
-    <sheet name="ProductSupplierGuarantee" sheetId="11" r:id="rId30"/>
-    <sheet name="PurchaseOrder" sheetId="20" r:id="rId31"/>
-    <sheet name="PurchaseOrderClearance" sheetId="21" r:id="rId32"/>
-    <sheet name="PurchaseOrderHistory" sheetId="22" r:id="rId33"/>
-    <sheet name="PurchaseOrderLineItem" sheetId="23" r:id="rId34"/>
-    <sheet name="PurchaseOrderPayment" sheetId="24" r:id="rId35"/>
-    <sheet name="Store" sheetId="2" r:id="rId36"/>
-    <sheet name="StoreAction" sheetId="13" r:id="rId37"/>
-    <sheet name="StoreActiveOnHand" sheetId="14" r:id="rId38"/>
-    <sheet name="StoreActivePriceList" sheetId="15" r:id="rId39"/>
-    <sheet name="StoreCalendar" sheetId="16" r:id="rId40"/>
-    <sheet name="StoreCalendarHistory" sheetId="17" r:id="rId41"/>
-    <sheet name="StoreDeliveryPerson" sheetId="18" r:id="rId42"/>
-    <sheet name="StoreValidRegionInfo" sheetId="19" r:id="rId43"/>
-    <sheet name="Supplier" sheetId="3" r:id="rId44"/>
+    <sheet name="ItemImage" sheetId="47" r:id="rId22"/>
+    <sheet name="Manufacture" sheetId="46" r:id="rId23"/>
+    <sheet name="Product" sheetId="1" r:id="rId24"/>
+    <sheet name="ProductBase" sheetId="8" r:id="rId25"/>
+    <sheet name="ProductBaseProductMap" sheetId="9" r:id="rId26"/>
+    <sheet name="ProductComment" sheetId="7" r:id="rId27"/>
+    <sheet name="ProductGroup" sheetId="6" r:id="rId28"/>
+    <sheet name="ProductPicture" sheetId="5" r:id="rId29"/>
+    <sheet name="ProductRate" sheetId="10" r:id="rId30"/>
+    <sheet name="ProductSupplierGuarantee" sheetId="11" r:id="rId31"/>
+    <sheet name="PurchaseOrder" sheetId="20" r:id="rId32"/>
+    <sheet name="PurchaseOrderClearance" sheetId="21" r:id="rId33"/>
+    <sheet name="PurchaseOrderHistory" sheetId="22" r:id="rId34"/>
+    <sheet name="PurchaseOrderLineItem" sheetId="23" r:id="rId35"/>
+    <sheet name="PurchaseOrderPayment" sheetId="24" r:id="rId36"/>
+    <sheet name="Store" sheetId="2" r:id="rId37"/>
+    <sheet name="StoreAction" sheetId="13" r:id="rId38"/>
+    <sheet name="StoreActiveOnHand" sheetId="14" r:id="rId39"/>
+    <sheet name="StoreActivePriceList" sheetId="15" r:id="rId40"/>
+    <sheet name="StoreCalendar" sheetId="16" r:id="rId41"/>
+    <sheet name="StoreCalendarHistory" sheetId="17" r:id="rId42"/>
+    <sheet name="StoreDeliveryPerson" sheetId="18" r:id="rId43"/>
+    <sheet name="StoreValidRegionInfo" sheetId="19" r:id="rId44"/>
+    <sheet name="Supplier" sheetId="3" r:id="rId45"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="380">
   <si>
     <t>MainAppProductId</t>
   </si>
@@ -884,9 +885,6 @@
     <t>BaseValueName</t>
   </si>
   <si>
-    <t>BasketTypeValueId</t>
-  </si>
-  <si>
     <t>BasketName</t>
   </si>
   <si>
@@ -983,9 +981,6 @@
     <t>CharTypeDesc</t>
   </si>
   <si>
-    <t>DefaultCharValueID</t>
-  </si>
-  <si>
     <t>CharGroupTypeInfoes</t>
   </si>
   <si>
@@ -1007,9 +1002,6 @@
     <t>CharValueID</t>
   </si>
   <si>
-    <t>CityRegionId</t>
-  </si>
-  <si>
     <t>ClearanceId</t>
   </si>
   <si>
@@ -1059,13 +1051,160 @@
   </si>
   <si>
     <t>FinalIsPrize</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>BasketTypeValueGuid</t>
+  </si>
+  <si>
+    <t>ForeignKey("Customer")</t>
+  </si>
+  <si>
+    <t>ForignKey("Product")</t>
+  </si>
+  <si>
+    <t>ForignKey("Basket")</t>
+  </si>
+  <si>
+    <t>CharTypes</t>
+  </si>
+  <si>
+    <t>Icollection-CharType</t>
+  </si>
+  <si>
+    <t>DefaultCharValueGuid</t>
+  </si>
+  <si>
+    <t>CharGroups</t>
+  </si>
+  <si>
+    <t>Icollection-CharGroup</t>
+  </si>
+  <si>
+    <t>ForeignKey("CharType")</t>
+  </si>
+  <si>
+    <t>CityRegion2Id</t>
+  </si>
+  <si>
+    <t>Guid?</t>
+  </si>
+  <si>
+    <t>Icollection-Store</t>
+  </si>
+  <si>
+    <t>CustomerInfoes</t>
+  </si>
+  <si>
+    <t>Icollection-Customer</t>
+  </si>
+  <si>
+    <t>CityRegion1</t>
+  </si>
+  <si>
+    <t>Icollection-CityRegion</t>
+  </si>
+  <si>
+    <t>ForeignKey("Cityregion2Id")</t>
+  </si>
+  <si>
+    <t>CityRegion2</t>
+  </si>
+  <si>
+    <t>NationalCode</t>
+  </si>
+  <si>
+    <t>ForeignKey("RegionInfo")</t>
+  </si>
+  <si>
+    <t>Column(order=0)</t>
+  </si>
+  <si>
+    <t>RegionInfoId</t>
+  </si>
+  <si>
+    <t>ForeignKey("RegionLevel1")</t>
+  </si>
+  <si>
+    <t>Column(order=1)</t>
+  </si>
+  <si>
+    <t>RegionLevel1Id</t>
+  </si>
+  <si>
+    <t>Column(order=2)</t>
+  </si>
+  <si>
+    <t>ForeignKey("RegionLevel2")</t>
+  </si>
+  <si>
+    <t>RegionLevel2Id</t>
+  </si>
+  <si>
+    <t>Column(order=3)</t>
+  </si>
+  <si>
+    <t>ForeignKey("RegionLevel3")</t>
+  </si>
+  <si>
+    <t>RegionLevel3Id</t>
+  </si>
+  <si>
+    <t>ForeignKey("RegionLevel4")</t>
+  </si>
+  <si>
+    <t>Column(order=4)</t>
+  </si>
+  <si>
+    <t>RegionLevel4Id</t>
+  </si>
+  <si>
+    <t>CustomerBaskets</t>
+  </si>
+  <si>
+    <t>Icollection-Basket</t>
+  </si>
+  <si>
+    <t>RegionInfo</t>
+  </si>
+  <si>
+    <t>RegionLevel1</t>
+  </si>
+  <si>
+    <t>RegionLevel2</t>
+  </si>
+  <si>
+    <t>RegionLevel3</t>
+  </si>
+  <si>
+    <t>RegionLevel4</t>
+  </si>
+  <si>
+    <t>TokenId</t>
+  </si>
+  <si>
+    <t>ImageName</t>
+  </si>
+  <si>
+    <t>ImageType</t>
+  </si>
+  <si>
+    <t>ManufactureName</t>
+  </si>
+  <si>
+    <t>ProductManufactures</t>
+  </si>
+  <si>
+    <t>ForeignKey("ProductGroup")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1107,13 +1246,45 @@
       <family val="1"/>
       <charset val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibiri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibiri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -1156,7 +1327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1192,7 +1363,75 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1501,8 +1740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1536,20 +1775,20 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="1">
+      <c r="A2" s="34">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="4"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="15">
       <c r="A3" s="1">
@@ -1590,7 +1829,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1657,7 +1896,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>21</v>
@@ -1689,7 +1928,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>28</v>
@@ -1707,7 +1946,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>28</v>
@@ -1743,7 +1982,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1778,106 +2017,106 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="1">
+      <c r="A2" s="34">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="4"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="15">
-      <c r="A3" s="1">
+      <c r="A3" s="34">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="4"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="15">
-      <c r="A4" s="1">
+      <c r="A4" s="34">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="4"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" ht="15">
-      <c r="A5" s="1">
+      <c r="A5" s="34">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="4"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" ht="15">
-      <c r="A6" s="1">
+      <c r="A6" s="34">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="4"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:6" ht="15">
-      <c r="A7" s="1">
+      <c r="A7" s="34">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="4"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6" ht="15">
-      <c r="A8" s="1">
+      <c r="A8" s="34">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="D8" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1887,17 +2126,17 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="3" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -1929,7 +2168,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>21</v>
@@ -1943,7 +2182,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>22</v>
@@ -1953,20 +2192,34 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="15">
-      <c r="A4" s="1">
+      <c r="A4" s="34">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="4"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="18"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1979,7 +2232,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2014,68 +2267,68 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="1">
+      <c r="A2" s="34">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="4"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="15">
-      <c r="A3" s="1">
+      <c r="A3" s="34">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="18"/>
+    </row>
+    <row r="4" spans="1:6" ht="15">
+      <c r="A4" s="34">
+        <v>3</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="15">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="18"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="34">
+        <v>4</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="C5" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="D5" s="39"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2085,10 +2338,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2127,7 +2380,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>22</v>
@@ -2137,64 +2390,78 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15">
-      <c r="A3" s="1">
+      <c r="A3" s="34">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="4"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="15">
-      <c r="A4" s="1">
+      <c r="A4" s="28">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="27"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="34">
+        <v>4</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="D5" s="39"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="28">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>340</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2204,7 +2471,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -2246,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>22</v>
@@ -2260,7 +2527,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>23</v>
@@ -2276,7 +2543,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>23</v>
@@ -2288,66 +2555,78 @@
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="15">
-      <c r="A5" s="1">
+      <c r="A5" s="28">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="4"/>
+      <c r="B5" s="24" t="s">
+        <v>341</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:6" ht="15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="14"/>
+      <c r="D6" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="E6" s="9" t="s">
         <v>29</v>
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1">
+    <row r="7" spans="1:6" ht="15">
+      <c r="A7" s="34">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="B7" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>98</v>
+        <v>305</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>101</v>
+        <v>305</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2357,16 +2636,16 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="27" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="3" customWidth="1"/>
@@ -2467,36 +2746,36 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="15">
-      <c r="A7" s="1">
+      <c r="A7" s="28">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="D7" s="33"/>
+      <c r="E7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="27"/>
+    </row>
+    <row r="8" spans="1:6" ht="15">
+      <c r="A8" s="34">
+        <v>7</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="15">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="D8" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1">
@@ -2505,12 +2784,66 @@
       <c r="B9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>80</v>
+      <c r="C9" s="27" t="s">
+        <v>344</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="28">
+        <v>9</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>346</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="28">
+        <v>10</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>348</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="28">
+        <v>11</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="28">
+        <v>12</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>350</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D13" s="33"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2562,7 +2895,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>21</v>
@@ -2578,7 +2911,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>73</v>
@@ -2594,7 +2927,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>22</v>
@@ -2608,7 +2941,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>111</v>
@@ -2624,7 +2957,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>21</v>
@@ -2640,7 +2973,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>21</v>
@@ -2659,16 +2992,16 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="3" customWidth="1"/>
@@ -2699,17 +3032,17 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="4"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="15">
       <c r="A3" s="1">
@@ -2781,7 +3114,7 @@
       <c r="C7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="40" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="11"/>
@@ -2805,49 +3138,49 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="4"/>
+      <c r="D9" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="36"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:6" ht="15">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="4"/>
+      <c r="D10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6" ht="15">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="4"/>
+      <c r="D11" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="41"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" ht="15">
       <c r="A12" s="1">
@@ -2878,108 +3211,356 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="15">
-      <c r="A14" s="1">
+      <c r="A14" s="28">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="24" t="s">
+        <v>351</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="27"/>
+    </row>
+    <row r="15" spans="1:6" ht="15">
+      <c r="A15" s="28">
+        <v>14</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>353</v>
+      </c>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="27"/>
+    </row>
+    <row r="16" spans="1:6" ht="15">
+      <c r="A16" s="28">
+        <v>15</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="38"/>
+      <c r="F16" s="27"/>
+    </row>
+    <row r="17" spans="1:6" ht="15">
+      <c r="A17" s="28">
+        <v>16</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>356</v>
+      </c>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="27"/>
+    </row>
+    <row r="18" spans="1:6" ht="15">
+      <c r="A18" s="28">
+        <v>17</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="38"/>
+      <c r="F18" s="27"/>
+    </row>
+    <row r="19" spans="1:6" ht="15">
+      <c r="A19" s="28">
+        <v>18</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>359</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>358</v>
+      </c>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="27"/>
+    </row>
+    <row r="20" spans="1:6" ht="15">
+      <c r="A20" s="28">
+        <v>19</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="38"/>
+      <c r="F20" s="27"/>
+    </row>
+    <row r="21" spans="1:6" ht="15">
+      <c r="A21" s="28">
+        <v>20</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>362</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>361</v>
+      </c>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="27"/>
+    </row>
+    <row r="22" spans="1:6" ht="15">
+      <c r="A22" s="28">
+        <v>21</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>363</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="38"/>
+      <c r="F22" s="27"/>
+    </row>
+    <row r="23" spans="1:6" ht="15">
+      <c r="A23" s="28">
+        <v>22</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>364</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="27"/>
+    </row>
+    <row r="24" spans="1:6" ht="15">
+      <c r="A24" s="28">
+        <v>23</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="38"/>
+      <c r="F24" s="27"/>
+    </row>
+    <row r="25" spans="1:6" ht="15">
+      <c r="A25" s="34">
+        <v>24</v>
+      </c>
+      <c r="B25" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C25" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" ht="15">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="D25" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="36"/>
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="1:6" ht="15">
+      <c r="A26" s="34">
+        <v>25</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C26" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" ht="15">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="7" t="s">
+      <c r="D26" s="16"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="1:6" ht="15">
+      <c r="A27" s="34">
+        <v>26</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C27" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" ht="15">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="7" t="s">
+      <c r="D27" s="16"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="1:6" ht="15">
+      <c r="A28" s="34">
+        <v>27</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C28" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" ht="15">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="7" t="s">
+      <c r="D28" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="36"/>
+      <c r="F28" s="18"/>
+    </row>
+    <row r="29" spans="1:6" ht="15">
+      <c r="A29" s="34">
+        <v>28</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C29" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" ht="15">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="7" t="s">
+      <c r="D29" s="16"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="18"/>
+    </row>
+    <row r="30" spans="1:6" ht="15">
+      <c r="A30" s="34">
+        <v>29</v>
+      </c>
+      <c r="B30" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C30" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" ht="15">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="7" t="s">
+      <c r="D30" s="16"/>
+      <c r="E30" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" spans="1:6" ht="15">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="4"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" ht="15">
+      <c r="A32" s="28">
+        <v>31</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>367</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="D32" s="33"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="28">
+        <v>32</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>369</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D33" s="33"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="28">
+        <v>33</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>370</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D34" s="33"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="28">
+        <v>34</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>371</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D35" s="33"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="28">
+        <v>35</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>372</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D36" s="33"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="28">
+        <v>36</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D37" s="33"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2991,8 +3572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3079,7 +3660,7 @@
       <c r="C5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="42" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="11"/>
@@ -3293,10 +3874,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3330,95 +3911,91 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="4"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="15">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="11"/>
+        <v>28</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="15">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="D4" s="9"/>
       <c r="E4" s="11"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="15">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="8"/>
       <c r="E5" s="11"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="15">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="D6" s="13"/>
+        <v>73</v>
+      </c>
+      <c r="D6" s="9"/>
       <c r="E6" s="11"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="15">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="D7" s="9"/>
+        <v>265</v>
+      </c>
+      <c r="D7" s="13"/>
       <c r="E7" s="11"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="15">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>267</v>
@@ -3429,10 +4006,10 @@
     </row>
     <row r="9" spans="1:6" ht="15">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>267</v>
@@ -3440,6 +4017,20 @@
       <c r="D9" s="9"/>
       <c r="E9" s="11"/>
       <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="15">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3507,7 +4098,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>22</v>
@@ -3521,7 +4112,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>22</v>
@@ -3555,7 +4146,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3610,7 +4201,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>28</v>
@@ -3624,7 +4215,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>22</v>
@@ -3638,7 +4229,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>27</v>
@@ -3657,17 +4248,17 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="3" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -3695,18 +4286,132 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="1">
+      <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="24" t="s">
+        <v>374</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="4"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="27"/>
+    </row>
+    <row r="3" spans="1:6" ht="15">
+      <c r="A3" s="28">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="27"/>
+    </row>
+    <row r="4" spans="1:6" ht="15">
+      <c r="A4" s="28">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>376</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15">
+      <c r="A2" s="34">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+    </row>
+    <row r="3" spans="1:6" ht="15">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3714,18 +4419,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="3" customWidth="1"/>
@@ -3753,18 +4458,18 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="1">
+      <c r="A2" s="34">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="4"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="15">
       <c r="A3" s="1">
@@ -3885,27 +4590,27 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="15">
-      <c r="A11" s="1">
+      <c r="A11" s="34">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="4"/>
+      <c r="D11" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="41"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" ht="15">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>22</v>
@@ -3915,34 +4620,28 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="15">
-      <c r="A13" s="1">
+      <c r="A13" s="28">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="4"/>
+      <c r="B13" s="24" t="s">
+        <v>379</v>
+      </c>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="27"/>
     </row>
     <row r="14" spans="1:6" ht="15">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>29</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D14" s="8"/>
       <c r="E14" s="13" t="s">
         <v>29</v>
       </c>
@@ -3953,12 +4652,14 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="E15" s="13" t="s">
         <v>29</v>
       </c>
@@ -3969,13 +4670,15 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" s="8"/>
-      <c r="E16" s="11"/>
+      <c r="E16" s="13" t="s">
+        <v>29</v>
+      </c>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="15">
@@ -3983,15 +4686,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="D17" s="8"/>
-      <c r="E17" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="E17" s="11"/>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="15">
@@ -3999,13 +4700,15 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D18" s="8"/>
-      <c r="E18" s="11"/>
+      <c r="E18" s="13" t="s">
+        <v>29</v>
+      </c>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="15">
@@ -4013,10 +4716,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="11"/>
@@ -4027,10 +4730,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="11"/>
@@ -4041,10 +4744,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="11"/>
@@ -4055,27 +4758,27 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="11"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" ht="15">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="4"/>
+      <c r="B23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="11"/>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6">
@@ -4083,14 +4786,28 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="D25" s="14"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4098,7 +4815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -4376,7 +5093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -4522,7 +5239,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -4716,7 +5433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -4922,7 +5639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -5035,170 +5752,6 @@
       <c r="D6" s="14"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="3.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15">
-      <c r="A1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" ht="15">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="15">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="15">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="15">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" ht="15">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5296,6 +5849,170 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="15">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="15">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="15">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="15">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="15">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5394,7 +6111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
@@ -6084,7 +6801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -6215,7 +6932,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -6415,7 +7132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
@@ -6762,7 +7479,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>50</v>
@@ -6791,7 +7508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -7021,7 +7738,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -7353,7 +8070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -7533,7 +8250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -7653,7 +8370,95 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15">
+      <c r="A2" s="34">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="18"/>
+    </row>
+    <row r="3" spans="1:6" ht="15">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="15">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -7791,95 +8596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="3.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15">
-      <c r="A1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" ht="15">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="15">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -8077,7 +8794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
@@ -8251,7 +8968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -8391,7 +9108,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -8495,7 +9212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -8619,16 +9336,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="3" customWidth="1"/>
@@ -8656,25 +9373,25 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="1">
+      <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="4"/>
+      <c r="B2" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:6" ht="15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>22</v>
@@ -8684,62 +9401,88 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="15">
-      <c r="A4" s="1">
+      <c r="A4" s="28">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="24" t="s">
+        <v>333</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+    </row>
+    <row r="5" spans="1:6" ht="15">
+      <c r="A5" s="28">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="15">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="4"/>
+      <c r="C5" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:6" ht="15">
-      <c r="A6" s="1">
+      <c r="A6" s="28">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="4"/>
+      <c r="B6" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="27"/>
     </row>
     <row r="7" spans="1:6" ht="15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>282</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="11"/>
       <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="15">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="15">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8749,10 +9492,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -8786,116 +9529,168 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="1">
+      <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="29" t="s">
+        <v>334</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="30"/>
+    </row>
+    <row r="3" spans="1:6" ht="15">
+      <c r="A3" s="28">
+        <v>2</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="30"/>
+    </row>
+    <row r="4" spans="1:6" ht="15">
+      <c r="A4" s="34">
+        <v>3</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="18"/>
+    </row>
+    <row r="5" spans="1:6" ht="15">
+      <c r="A5" s="28">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="27"/>
+    </row>
+    <row r="6" spans="1:6" ht="15">
+      <c r="A6" s="34">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="18"/>
+    </row>
+    <row r="7" spans="1:6" ht="15">
+      <c r="A7" s="34">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="18"/>
+    </row>
+    <row r="8" spans="1:6" ht="15">
+      <c r="A8" s="28">
+        <v>7</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="27"/>
+    </row>
+    <row r="9" spans="1:6" ht="15">
+      <c r="A9" s="35">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" ht="15">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="15">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="15">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="15">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="4" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="15">
+      <c r="A10" s="35">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="15">
+      <c r="A11" s="28">
+        <v>10</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="27"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="35">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8946,7 +9741,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>21</v>
@@ -8992,7 +9787,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>22</v>
@@ -9006,7 +9801,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>73</v>
@@ -9022,7 +9817,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>22</v>
@@ -9036,7 +9831,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>111</v>
@@ -9052,7 +9847,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>50</v>
@@ -9126,7 +9921,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>22</v>
@@ -9140,7 +9935,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>28</v>
@@ -9156,10 +9951,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="11"/>
@@ -9170,10 +9965,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -9204,7 +9999,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9267,7 +10062,7 @@
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15">
@@ -9307,7 +10102,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>28</v>
@@ -9323,7 +10118,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>28</v>

</xml_diff>